<commit_message>
Update on 2025/12/12 13:37:06.03
</commit_message>
<xml_diff>
--- a/資料/ToDoリストの手順書.xlsx
+++ b/資料/ToDoリストの手順書.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\delphi\初めてのアプリ\Todoリスト 修正版\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\delphi\Mycreate_app\資料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8141EDFA-C008-426C-884E-5BAA55D0518E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53269A7D-A7C8-4344-9E25-FC5C84AF10AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{71441DE0-A21D-498E-87EF-DC4DEA628ADE}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{71441DE0-A21D-498E-87EF-DC4DEA628ADE}"/>
   </bookViews>
   <sheets>
     <sheet name="概要" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>作成したアプリ</t>
     <rPh sb="0" eb="2">
@@ -64,32 +64,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>タスクを一目でわかるようにしたいため。</t>
-    <rPh sb="4" eb="6">
-      <t>ヒトメ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>初めて作るので、自分でコードが理解できる範囲のものを作成したかったため。</t>
-    <rPh sb="0" eb="1">
-      <t>ハジ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>ツク</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ジブン</t>
-    </rPh>
-    <rPh sb="15" eb="17">
-      <t>リカイ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>サクセイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>概要</t>
     <rPh sb="0" eb="2">
       <t>ガイヨウ</t>
@@ -216,82 +190,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>１．赤枠の検索欄に打ち込まれたキーワードを検索する。</t>
-    <rPh sb="2" eb="4">
-      <t>アカワク</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ケンサク</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ラン</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ウ</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ケンサク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>３．文字が入力されるたびにToDoリストの中身を参照する。</t>
-    <rPh sb="2" eb="4">
-      <t>モジ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>ニュウリョク</t>
-    </rPh>
-    <rPh sb="21" eb="23">
-      <t>ナカミ</t>
-    </rPh>
-    <rPh sb="24" eb="26">
-      <t>サンショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>２．キーワードが撃ち込まれたらToDoリストは空にする。</t>
-    <rPh sb="8" eb="9">
-      <t>ウ</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>カラ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>４．テキスト、優先度、カテゴリ、期限の中から一致する文字列が含まれるものをToDoリストに表示。</t>
-    <rPh sb="7" eb="10">
-      <t>ユウセンド</t>
-    </rPh>
-    <rPh sb="16" eb="18">
-      <t>キゲン</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>ナカ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>イッチ</t>
-    </rPh>
-    <rPh sb="26" eb="29">
-      <t>モジレツ</t>
-    </rPh>
-    <rPh sb="30" eb="31">
-      <t>フク</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>５．追加ボタンクリックまたはEnterキーを押下することで新規追加、編集を実行する。</t>
     <rPh sb="2" eb="4">
       <t>ツイカ</t>
@@ -547,58 +445,91 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ToDoの追加、編集、検索ができる。</t>
+    <t>１．赤枠の検索欄に入力されたキーワードを検索する。</t>
+    <rPh sb="2" eb="4">
+      <t>アカワク</t>
+    </rPh>
     <rPh sb="5" eb="7">
-      <t>ツイカ</t>
-    </rPh>
-    <rPh sb="8" eb="10">
-      <t>ヘンシュウ</t>
-    </rPh>
-    <rPh sb="11" eb="13">
       <t>ケンサク</t>
     </rPh>
+    <rPh sb="7" eb="8">
+      <t>ラン</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ケンサク</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>また、JSONファイルにデータを保存することで、アプリを終了しても保存と復元が可能。</t>
+    <t>２．テキスト、優先度、カテゴリ、期限の中から一致する文字列が含まれるものをToDoリストに表示。</t>
+    <rPh sb="7" eb="10">
+      <t>ユウセンド</t>
+    </rPh>
     <rPh sb="16" eb="18">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="28" eb="30">
-      <t>シュウリョウ</t>
-    </rPh>
-    <rPh sb="33" eb="35">
-      <t>ホゾン</t>
-    </rPh>
-    <rPh sb="36" eb="38">
-      <t>フクゲン</t>
-    </rPh>
-    <rPh sb="39" eb="41">
-      <t>カノウ</t>
+      <t>キゲン</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>イッチ</t>
+    </rPh>
+    <rPh sb="26" eb="29">
+      <t>モジレツ</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヒョウジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>優先度、カテゴリ、期限を付けることでタスクの細分化を実施。</t>
+    <t>今後の業今後の業務でタスクの内容をひと目で把握できるようにするためです。務においてタスクを一目でわかるようにしたいため。</t>
     <rPh sb="0" eb="2">
-      <t>ユウセン</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ド</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>キゲン</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ツ</t>
-    </rPh>
-    <rPh sb="22" eb="25">
-      <t>サイブンカ</t>
-    </rPh>
-    <rPh sb="26" eb="28">
-      <t>ジッシ</t>
+      <t>コンゴ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ギョウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>コンゴ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ギョウム</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ナイヨウ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>メ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>ハアク</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>ツトム</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>ヒトメ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>また、今回が初めての作成となるため、自分でコードを理解しながら扱える範囲で作りたいと考えています</t>
+  </si>
+  <si>
+    <t>本ツールでは、ToDoリストへの追加・編集・検索が可能です。</t>
+  </si>
+  <si>
+    <t>タスクには優先度・カテゴリ・期限を設定でき、より細分化した管理が行えます。</t>
+  </si>
+  <si>
+    <t>さらに、データはJSONファイルに保存されるため、アプリ終了後も内容を保持し、再起動時に復元することができます。</t>
   </si>
 </sst>
 </file>
@@ -3004,7 +2935,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -3026,37 +2957,37 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3068,37 +2999,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46BD06BB-D942-4636-A49C-F3925C129132}">
-  <dimension ref="B20:C24"/>
+  <dimension ref="B20:C22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="C24" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -3112,7 +3033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E76FA48-5488-470C-9CF3-929CD363479C}">
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
@@ -3120,50 +3041,50 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C27" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3177,7 +3098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA6332D-BD50-41B8-B38E-F832A064688E}">
   <dimension ref="B20:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -3185,17 +3106,17 @@
   <sheetData>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -3217,22 +3138,22 @@
   <sheetData>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3254,22 +3175,22 @@
   <sheetData>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C23" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3291,17 +3212,17 @@
   <sheetData>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3315,7 +3236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4708AC-7B94-4787-B7EF-A291503E8D7B}">
   <dimension ref="B20:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -3323,17 +3244,17 @@
   <sheetData>
     <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C21" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="C22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>